<commit_message>
Hybrid Filter Options Implemented and Working
</commit_message>
<xml_diff>
--- a/NewLegacyBBDD/computers.xlsx
+++ b/NewLegacyBBDD/computers.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4772574B-C511-4B68-853B-239136E5E97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="435">
   <si>
     <t>Site</t>
   </si>
@@ -754,13 +755,583 @@
   </si>
   <si>
     <t>PcModel</t>
+  </si>
+  <si>
+    <t>Illescas</t>
+  </si>
+  <si>
+    <t>LIDL</t>
+  </si>
+  <si>
+    <t>ESDT8CC128243V</t>
+  </si>
+  <si>
+    <t>HP ProDesk 600 G7</t>
+  </si>
+  <si>
+    <t>8CC128243V</t>
+  </si>
+  <si>
+    <t>Emilio Lara Montero</t>
+  </si>
+  <si>
+    <t>montoroe</t>
+  </si>
+  <si>
+    <t>UPONOR</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VC9</t>
+  </si>
+  <si>
+    <t>HP ProDesk 600 G8</t>
+  </si>
+  <si>
+    <t>8CC2122VC9</t>
+  </si>
+  <si>
+    <t>Mercedes Ibañez</t>
+  </si>
+  <si>
+    <t>ibanezm</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VCT</t>
+  </si>
+  <si>
+    <t>HP ProDesk 600 G9</t>
+  </si>
+  <si>
+    <t>8CC2122VCT</t>
+  </si>
+  <si>
+    <t>Pilar Cámara</t>
+  </si>
+  <si>
+    <t>camarapi</t>
+  </si>
+  <si>
+    <t>Borox</t>
+  </si>
+  <si>
+    <t>SONAE</t>
+  </si>
+  <si>
+    <t>ESDT8CC9141X8T</t>
+  </si>
+  <si>
+    <t>8CC9141X8T</t>
+  </si>
+  <si>
+    <t>Gabriel Martin</t>
+  </si>
+  <si>
+    <t>marting</t>
+  </si>
+  <si>
+    <t>ESDT8CC03716DW</t>
+  </si>
+  <si>
+    <t>8CC03716DW</t>
+  </si>
+  <si>
+    <t>Matilde Fernandez</t>
+  </si>
+  <si>
+    <t>fernandezma</t>
+  </si>
+  <si>
+    <t>ESDT8CC9141X8W</t>
+  </si>
+  <si>
+    <t>8CC9141X8W</t>
+  </si>
+  <si>
+    <t>Belén Sáncehz</t>
+  </si>
+  <si>
+    <t>sanchezb</t>
+  </si>
+  <si>
+    <t>Zamudio</t>
+  </si>
+  <si>
+    <t>ITP Zamudio</t>
+  </si>
+  <si>
+    <t>EDT8CC9084G0T</t>
+  </si>
+  <si>
+    <t>HP ProDesk 600 G4</t>
+  </si>
+  <si>
+    <t>8CC9084G0T</t>
+  </si>
+  <si>
+    <t>Juan Ignacio Gonzalez de Prado</t>
+  </si>
+  <si>
+    <t>pradoj</t>
+  </si>
+  <si>
+    <t>ESDT5CG9392NGN</t>
+  </si>
+  <si>
+    <t>5CG9392NGN</t>
+  </si>
+  <si>
+    <t>Iker Aldamiz</t>
+  </si>
+  <si>
+    <t>aldamizi</t>
+  </si>
+  <si>
+    <t>ESLT5CG1026CWY</t>
+  </si>
+  <si>
+    <t>5CG1026CWY</t>
+  </si>
+  <si>
+    <t>Edgar Rojas</t>
+  </si>
+  <si>
+    <t>rojasedg</t>
+  </si>
+  <si>
+    <t>ESLT5CG0030V82</t>
+  </si>
+  <si>
+    <t>5CG0030V82</t>
+  </si>
+  <si>
+    <t>Oihane Perez</t>
+  </si>
+  <si>
+    <t>PerezOi</t>
+  </si>
+  <si>
+    <t>ESLTPC074B9T</t>
+  </si>
+  <si>
+    <t>Lenovo Thinkpad T450</t>
+  </si>
+  <si>
+    <t>PC074B9T</t>
+  </si>
+  <si>
+    <t>Borja nunez</t>
+  </si>
+  <si>
+    <t>nunezbo</t>
+  </si>
+  <si>
+    <t>ESLTPC0DJGRT</t>
+  </si>
+  <si>
+    <t>PC0DJGRT</t>
+  </si>
+  <si>
+    <t>Daniel Sole</t>
+  </si>
+  <si>
+    <t>soled</t>
+  </si>
+  <si>
+    <t>ESLT5CG1423PCZ</t>
+  </si>
+  <si>
+    <t>5CG1423PCZ</t>
+  </si>
+  <si>
+    <t>ESLT5CG14376CL</t>
+  </si>
+  <si>
+    <t>5CG14376CL</t>
+  </si>
+  <si>
+    <t>Ontigola</t>
+  </si>
+  <si>
+    <t>AMAZON HAZMAT</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VCJ</t>
+  </si>
+  <si>
+    <t>HP EliteDesk 805 G5</t>
+  </si>
+  <si>
+    <t>8CC2061KNY</t>
+  </si>
+  <si>
+    <t>AMAZON</t>
+  </si>
+  <si>
+    <t>HP EliteDesk 805 G6</t>
+  </si>
+  <si>
+    <t>8CC2122VCJ</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VCB</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VC8</t>
+  </si>
+  <si>
+    <t>8CC2122VCB</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VCN</t>
+  </si>
+  <si>
+    <t>8CC2122VC8</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VBV</t>
+  </si>
+  <si>
+    <t>8CC2122VCN</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VC2</t>
+  </si>
+  <si>
+    <t>8CC2122VBV</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VBW</t>
+  </si>
+  <si>
+    <t>8CC2122VC2</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VC4</t>
+  </si>
+  <si>
+    <t>8CC2122VBW</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VBQ</t>
+  </si>
+  <si>
+    <t>8CC2122VC4</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VBP</t>
+  </si>
+  <si>
+    <t>8CC2122VBQ</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VBT</t>
+  </si>
+  <si>
+    <t>8CC2122VBP</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VC0</t>
+  </si>
+  <si>
+    <t>8CC2122VBT</t>
+  </si>
+  <si>
+    <t>ESDT8CC2122VC3</t>
+  </si>
+  <si>
+    <t>8CC2122VC0</t>
+  </si>
+  <si>
+    <t>ESDT8CC2061KNR</t>
+  </si>
+  <si>
+    <t>8CC2122VC3</t>
+  </si>
+  <si>
+    <t>ESDT8CC9170KBK</t>
+  </si>
+  <si>
+    <t>8CC2061KNR</t>
+  </si>
+  <si>
+    <t>ESDT8CC2061KP3</t>
+  </si>
+  <si>
+    <t>HP Elitedesk 705 G4</t>
+  </si>
+  <si>
+    <t>8CC9170KBK</t>
+  </si>
+  <si>
+    <t>ESDT8CC14838LQ</t>
+  </si>
+  <si>
+    <t>8CC2061KP3</t>
+  </si>
+  <si>
+    <t>ESDT8CC30716DX</t>
+  </si>
+  <si>
+    <t>HP ELITEDESK 845G8</t>
+  </si>
+  <si>
+    <t>8CC14838LQ</t>
+  </si>
+  <si>
+    <t>ESDT8CG90223MFW</t>
+  </si>
+  <si>
+    <t>8CC30716DX</t>
+  </si>
+  <si>
+    <t>AMAZON BWS</t>
+  </si>
+  <si>
+    <t>ESLT5CG24007V5</t>
+  </si>
+  <si>
+    <t>HP Elitebook 845 G8</t>
+  </si>
+  <si>
+    <t>5CG24007V5</t>
+  </si>
+  <si>
+    <t>ESLT5CG24007V7</t>
+  </si>
+  <si>
+    <t>5CG24007V7</t>
+  </si>
+  <si>
+    <t>ESLT5CG24007V4</t>
+  </si>
+  <si>
+    <t>5CG24007V4</t>
+  </si>
+  <si>
+    <t>ESLT5CG2241ZML</t>
+  </si>
+  <si>
+    <t>5CG2241ZML</t>
+  </si>
+  <si>
+    <t>ESLT5CG2241ZMR</t>
+  </si>
+  <si>
+    <t>5CG2241ZMR</t>
+  </si>
+  <si>
+    <t>ESLT5CG2241ZMT</t>
+  </si>
+  <si>
+    <t>Elitebook 845 G8</t>
+  </si>
+  <si>
+    <t>5CG2471XKC</t>
+  </si>
+  <si>
+    <t>ESLT5CG2471XK6</t>
+  </si>
+  <si>
+    <t>5CG2471XK6</t>
+  </si>
+  <si>
+    <t>ESLT5CG2471XK8</t>
+  </si>
+  <si>
+    <t>5CG2471XK8</t>
+  </si>
+  <si>
+    <t>ESLT5CG2471XK7</t>
+  </si>
+  <si>
+    <t>5CG2471XK7</t>
+  </si>
+  <si>
+    <t>ESLT5CG2471XKB</t>
+  </si>
+  <si>
+    <t>5CG2471XKB</t>
+  </si>
+  <si>
+    <t>ESLT5CG2471XKF</t>
+  </si>
+  <si>
+    <t>5CG2471XKF</t>
+  </si>
+  <si>
+    <t>ESLT5CG2471XKH</t>
+  </si>
+  <si>
+    <t>5CG2471XKH</t>
+  </si>
+  <si>
+    <t>ESLT5CG2471XK9</t>
+  </si>
+  <si>
+    <t>5CG2471XK9</t>
+  </si>
+  <si>
+    <t>ESLT5CG2471XKG</t>
+  </si>
+  <si>
+    <t>5CG2471XKG</t>
+  </si>
+  <si>
+    <t>ESLT5CG2471XKD</t>
+  </si>
+  <si>
+    <t>5CG2471XKD</t>
+  </si>
+  <si>
+    <t>AMAZON ILLESCAS</t>
+  </si>
+  <si>
+    <t>ESDT8CC128243S</t>
+  </si>
+  <si>
+    <t>8CC128243S</t>
+  </si>
+  <si>
+    <t>Cristina del Cerro</t>
+  </si>
+  <si>
+    <t>delcerroc</t>
+  </si>
+  <si>
+    <t>ESDT8CC128243R</t>
+  </si>
+  <si>
+    <t>HP EliteDesk 805 G7</t>
+  </si>
+  <si>
+    <t>8CC128243R</t>
+  </si>
+  <si>
+    <t>Sara Lopez Azores</t>
+  </si>
+  <si>
+    <t>slopez</t>
+  </si>
+  <si>
+    <t>OXFORD</t>
+  </si>
+  <si>
+    <t>ESDT8CC9023MG3</t>
+  </si>
+  <si>
+    <t>8CC9023MG3</t>
+  </si>
+  <si>
+    <t>Raúl Torres / José Luís Merino</t>
+  </si>
+  <si>
+    <t>torrer</t>
+  </si>
+  <si>
+    <t>AMAZON PESG</t>
+  </si>
+  <si>
+    <t>ESLT5CG30317SV</t>
+  </si>
+  <si>
+    <t>5CG30317SV</t>
+  </si>
+  <si>
+    <t>David Lopez / Estefania Velasco</t>
+  </si>
+  <si>
+    <t>lopezda</t>
+  </si>
+  <si>
+    <t>00768OW23006845</t>
+  </si>
+  <si>
+    <t>ESLT5CG30317ST</t>
+  </si>
+  <si>
+    <t>5CG30317ST</t>
+  </si>
+  <si>
+    <t>Ruben González</t>
+  </si>
+  <si>
+    <t>rubengo</t>
+  </si>
+  <si>
+    <t>ESLTYN007F8Y</t>
+  </si>
+  <si>
+    <t>ideapad s540</t>
+  </si>
+  <si>
+    <t>YN007F8Y</t>
+  </si>
+  <si>
+    <t>FORMACION</t>
+  </si>
+  <si>
+    <t>ESLTR90WTVMK</t>
+  </si>
+  <si>
+    <t>LENOVO L13</t>
+  </si>
+  <si>
+    <t>R90WTVMK</t>
+  </si>
+  <si>
+    <t>GROUND</t>
+  </si>
+  <si>
+    <t>ESDT8CG9490464</t>
+  </si>
+  <si>
+    <t>HP Elitedesk 705 G4 35w</t>
+  </si>
+  <si>
+    <t>8CG9490464</t>
+  </si>
+  <si>
+    <t>Ramón Vela</t>
+  </si>
+  <si>
+    <t>velar</t>
+  </si>
+  <si>
+    <t>ESDT8CC9115M0L</t>
+  </si>
+  <si>
+    <t>8CC9115M0L</t>
+  </si>
+  <si>
+    <t>Yessica Hermida</t>
+  </si>
+  <si>
+    <t>hermiday</t>
+  </si>
+  <si>
+    <t>ESDTC14838LL</t>
+  </si>
+  <si>
+    <t>HP ProDesk 600 G5</t>
+  </si>
+  <si>
+    <t>8CC14838LL</t>
+  </si>
+  <si>
+    <t>HP ProDesk 600 G6</t>
+  </si>
+  <si>
+    <t>Patricia Alonso</t>
+  </si>
+  <si>
+    <t>alonsop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -843,6 +1414,38 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF363636"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -897,7 +1500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -924,6 +1527,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1203,22 +1820,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="17.6328125" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="35.85546875" customWidth="1"/>
+    <col min="9" max="9" width="48.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1247,7 +1867,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1274,7 +1894,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1301,7 +1921,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1330,7 +1950,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1359,7 +1979,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1388,7 +2008,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1417,7 +2037,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1446,7 +2066,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1475,7 +2095,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1504,7 +2124,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -1533,7 +2153,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
@@ -1562,7 +2182,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1589,7 +2209,7 @@
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1614,7 +2234,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1643,7 +2263,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1656,7 +2276,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>8</v>
       </c>
@@ -1683,7 +2303,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
@@ -1710,7 +2330,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -1737,7 +2357,7 @@
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>8</v>
       </c>
@@ -1764,7 +2384,7 @@
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -1789,7 +2409,7 @@
       </c>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1818,7 +2438,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -1847,7 +2467,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -1872,7 +2492,7 @@
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -1901,7 +2521,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>8</v>
       </c>
@@ -1926,7 +2546,7 @@
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>8</v>
       </c>
@@ -1953,7 +2573,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>8</v>
       </c>
@@ -1978,7 +2598,7 @@
       </c>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>8</v>
       </c>
@@ -2003,7 +2623,7 @@
       </c>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>8</v>
       </c>
@@ -2028,7 +2648,7 @@
       </c>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -2053,7 +2673,7 @@
       </c>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -2078,7 +2698,7 @@
       </c>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -2103,7 +2723,7 @@
       </c>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -2128,7 +2748,7 @@
       </c>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -2153,7 +2773,7 @@
       </c>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>8</v>
       </c>
@@ -2178,7 +2798,7 @@
       </c>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
@@ -2203,7 +2823,7 @@
       </c>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>8</v>
       </c>
@@ -2228,7 +2848,7 @@
       </c>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>8</v>
       </c>
@@ -2253,7 +2873,7 @@
       </c>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>8</v>
       </c>
@@ -2278,7 +2898,7 @@
       </c>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>8</v>
       </c>
@@ -2303,7 +2923,7 @@
       </c>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>8</v>
       </c>
@@ -2328,7 +2948,7 @@
       </c>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>8</v>
       </c>
@@ -2353,7 +2973,7 @@
       </c>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>8</v>
       </c>
@@ -2378,7 +2998,7 @@
       </c>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>8</v>
       </c>
@@ -2405,7 +3025,7 @@
       </c>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>8</v>
       </c>
@@ -2430,7 +3050,7 @@
       </c>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>8</v>
       </c>
@@ -2455,7 +3075,7 @@
       </c>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>8</v>
       </c>
@@ -2480,7 +3100,7 @@
       </c>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>8</v>
       </c>
@@ -2509,7 +3129,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>8</v>
       </c>
@@ -2536,7 +3156,1583 @@
       </c>
       <c r="I50" s="2"/>
     </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="F51" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H51" s="18"/>
+      <c r="I51" s="19"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F52" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>318</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F54" s="18" t="s">
+        <v>319</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F55" s="18" t="s">
+        <v>321</v>
+      </c>
+      <c r="G55" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H55" s="18"/>
+      <c r="I55" s="20"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F56" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="G56" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F57" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="G57" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F58" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="G58" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F59" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="G59" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H59" s="18"/>
+      <c r="I59" s="18"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F60" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="G60" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H60" s="18"/>
+      <c r="I60" s="21"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B61" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F61" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="G61" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H61" s="18"/>
+      <c r="I61" s="21"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F62" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="G62" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F63" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="G63" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H63" s="18"/>
+      <c r="I63" s="18"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B64" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E64" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F64" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="G64" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H64" s="18"/>
+      <c r="I64" s="19"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B65" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F65" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="G65" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H65" s="19"/>
+      <c r="I65" s="18"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B66" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F66" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="G66" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E67" s="18" t="s">
+        <v>345</v>
+      </c>
+      <c r="F67" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="G67" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H67" s="19"/>
+      <c r="I67" s="18"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B68" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F68" s="22" t="s">
+        <v>348</v>
+      </c>
+      <c r="G68" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H68" s="19"/>
+      <c r="I68" s="18"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B69" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="F69" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="G69" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H69" s="19"/>
+      <c r="I69" s="18"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="18" t="s">
+        <v>350</v>
+      </c>
+      <c r="F70" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="G70" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H70" s="18"/>
+      <c r="I70" s="18"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="F71" s="23" t="s">
+        <v>357</v>
+      </c>
+      <c r="G71" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H71" s="19"/>
+      <c r="I71" s="19"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B72" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="F72" s="23" t="s">
+        <v>359</v>
+      </c>
+      <c r="G72" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H72" s="19"/>
+      <c r="I72" s="19"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>360</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="F73" s="23" t="s">
+        <v>361</v>
+      </c>
+      <c r="G73" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>362</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E74" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="F74" s="23" t="s">
+        <v>363</v>
+      </c>
+      <c r="G74" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H74" s="19"/>
+      <c r="I74" s="19"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E75" s="23" t="s">
+        <v>356</v>
+      </c>
+      <c r="F75" s="23" t="s">
+        <v>365</v>
+      </c>
+      <c r="G75" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H75" s="18"/>
+      <c r="I75" s="18"/>
+    </row>
+    <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>366</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E76" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="F76" s="23" t="s">
+        <v>368</v>
+      </c>
+      <c r="G76" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>369</v>
+      </c>
+      <c r="D77" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E77" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="F77" s="23" t="s">
+        <v>370</v>
+      </c>
+      <c r="G77" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H77" s="18"/>
+      <c r="I77" s="18"/>
+    </row>
+    <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B78" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C78" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="D78" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="F78" s="23" t="s">
+        <v>372</v>
+      </c>
+      <c r="G78" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H78" s="18"/>
+      <c r="I78" s="18"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B79" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="D79" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="F79" s="23" t="s">
+        <v>374</v>
+      </c>
+      <c r="G79" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H79" s="18"/>
+      <c r="I79" s="18"/>
+    </row>
+    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>375</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E80" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="F80" s="23" t="s">
+        <v>376</v>
+      </c>
+      <c r="G80" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H80" s="18"/>
+      <c r="I80" s="18"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B81" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>377</v>
+      </c>
+      <c r="D81" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E81" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="F81" s="23" t="s">
+        <v>378</v>
+      </c>
+      <c r="G81" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H81" s="18"/>
+      <c r="I81" s="18"/>
+    </row>
+    <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B82" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>379</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="F82" s="23" t="s">
+        <v>380</v>
+      </c>
+      <c r="G82" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H82" s="18"/>
+      <c r="I82" s="18"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B83" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>381</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E83" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="F83" s="23" t="s">
+        <v>382</v>
+      </c>
+      <c r="G83" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+    </row>
+    <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B84" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="D84" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E84" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="F84" s="23" t="s">
+        <v>384</v>
+      </c>
+      <c r="G84" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="B85" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E85" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="F85" s="23" t="s">
+        <v>386</v>
+      </c>
+      <c r="G85" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="H85" s="18"/>
+      <c r="I85" s="18"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B86" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="D86" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E86" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="F86" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="G86" s="18" t="s">
+        <v>390</v>
+      </c>
+      <c r="H86" s="18" t="s">
+        <v>391</v>
+      </c>
+      <c r="I86" s="18"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B87" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="C87" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="D87" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="F87" s="25" t="s">
+        <v>249</v>
+      </c>
+      <c r="G87" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="H87" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="I87" s="18"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B88" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="D88" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E88" s="18" t="s">
+        <v>393</v>
+      </c>
+      <c r="F88" s="18" t="s">
+        <v>394</v>
+      </c>
+      <c r="G88" s="18" t="s">
+        <v>395</v>
+      </c>
+      <c r="H88" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="I88" s="18"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B89" s="18" t="s">
+        <v>397</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>398</v>
+      </c>
+      <c r="D89" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="F89" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="G89" s="18" t="s">
+        <v>400</v>
+      </c>
+      <c r="H89" s="18" t="s">
+        <v>401</v>
+      </c>
+      <c r="I89" s="18"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B90" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="C90" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="D90" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E90" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="F90" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="G90" s="18" t="s">
+        <v>405</v>
+      </c>
+      <c r="H90" s="18" t="s">
+        <v>406</v>
+      </c>
+      <c r="I90" s="18" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B91" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="C91" s="18" t="s">
+        <v>408</v>
+      </c>
+      <c r="D91" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E91" s="18" t="s">
+        <v>367</v>
+      </c>
+      <c r="F91" s="18" t="s">
+        <v>409</v>
+      </c>
+      <c r="G91" s="18" t="s">
+        <v>410</v>
+      </c>
+      <c r="H91" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="I91" s="18" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B92" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="C92" s="18" t="s">
+        <v>412</v>
+      </c>
+      <c r="D92" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E92" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="F92" s="18" t="s">
+        <v>414</v>
+      </c>
+      <c r="G92" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="H92" s="18"/>
+      <c r="I92" s="18"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B93" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="C93" s="18" t="s">
+        <v>416</v>
+      </c>
+      <c r="D93" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E93" s="18" t="s">
+        <v>417</v>
+      </c>
+      <c r="F93" s="18" t="s">
+        <v>418</v>
+      </c>
+      <c r="G93" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="H93" s="18"/>
+      <c r="I93" s="18"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B94" s="18" t="s">
+        <v>419</v>
+      </c>
+      <c r="C94" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="D94" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E94" s="18" t="s">
+        <v>421</v>
+      </c>
+      <c r="F94" s="18" t="s">
+        <v>422</v>
+      </c>
+      <c r="G94" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="H94" s="18" t="s">
+        <v>424</v>
+      </c>
+      <c r="I94" s="18"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B95" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>425</v>
+      </c>
+      <c r="D95" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E95" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="F95" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="G95" s="18" t="s">
+        <v>427</v>
+      </c>
+      <c r="H95" s="18" t="s">
+        <v>428</v>
+      </c>
+      <c r="I95" s="18"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B96" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="C96" s="18" t="s">
+        <v>429</v>
+      </c>
+      <c r="D96" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E96" s="18" t="s">
+        <v>430</v>
+      </c>
+      <c r="F96" s="18" t="s">
+        <v>431</v>
+      </c>
+      <c r="G96" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="H96" s="18"/>
+      <c r="I96" s="18"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B97" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>392</v>
+      </c>
+      <c r="D97" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E97" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="F97" s="18" t="s">
+        <v>394</v>
+      </c>
+      <c r="G97" s="18" t="s">
+        <v>433</v>
+      </c>
+      <c r="H97" s="18" t="s">
+        <v>434</v>
+      </c>
+      <c r="I97" s="18"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B98" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="C98" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="D98" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E98" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="F98" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="G98" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="H98" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="I98" s="18"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B99" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="D99" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E99" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="F99" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="G99" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="H99" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="I99" s="18"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="B100" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="D100" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E100" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="F100" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="G100" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="H100" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="I100" s="18"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="B101" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="C101" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="D101" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E101" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="F101" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="G101" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="H101" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="I101" s="18"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="B102" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="C102" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="D102" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E102" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="F102" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="G102" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="H102" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="I102" s="18"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="B103" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="D103" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E103" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="F103" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="G103" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="H103" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="I103" s="18"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="B104" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C104" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="D104" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E104" s="18" t="s">
+        <v>280</v>
+      </c>
+      <c r="F104" s="18" t="s">
+        <v>281</v>
+      </c>
+      <c r="G104" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="H104" s="18" t="s">
+        <v>283</v>
+      </c>
+      <c r="I104" s="18"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="B105" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C105" s="18" t="s">
+        <v>284</v>
+      </c>
+      <c r="D105" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E105" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="F105" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="G105" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="H105" s="18" t="s">
+        <v>287</v>
+      </c>
+      <c r="I105" s="18"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="B106" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C106" s="18" t="s">
+        <v>288</v>
+      </c>
+      <c r="D106" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E106" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="F106" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="G106" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="H106" s="18" t="s">
+        <v>291</v>
+      </c>
+      <c r="I106" s="18"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="B107" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C107" s="18" t="s">
+        <v>292</v>
+      </c>
+      <c r="D107" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E107" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F107" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="G107" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="H107" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="I107" s="18"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="B108" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C108" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="D108" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E108" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="F108" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="G108" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="H108" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="I108" s="18"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="B109" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C109" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="D109" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E109" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="F109" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="G109" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="H109" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="I109" s="18"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="B110" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C110" s="18" t="s">
+        <v>305</v>
+      </c>
+      <c r="D110" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E110" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F110" s="18" t="s">
+        <v>306</v>
+      </c>
+      <c r="G110" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="H110" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="I110" s="18"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="B111" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C111" s="18" t="s">
+        <v>307</v>
+      </c>
+      <c r="D111" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E111" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F111" s="18" t="s">
+        <v>308</v>
+      </c>
+      <c r="G111" s="18" t="s">
+        <v>303</v>
+      </c>
+      <c r="H111" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="I111" s="18"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>